<commit_message>
ADD: .spf pin map
</commit_message>
<xml_diff>
--- a/bist/atpg_pat_converter/PinFunc/PIs.xlsx
+++ b/bist/atpg_pat_converter/PinFunc/PIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luca/Documents/VirtualShared/testing/RISCV_LBIST/bist/atpg_pat_converter/PinFunc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B97329D-0B97-6840-BF19-06C2FA684ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83704488-8D73-2147-9C0F-F58510CACE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25440" windowHeight="14400" xr2:uid="{C32979EF-4B37-0B40-98B1-A31D6BD3C0AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{C32979EF-4B37-0B40-98B1-A31D6BD3C0AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -838,9 +838,6 @@
     <t>FIXED AT 'test_rst_g' in test_mode</t>
   </si>
   <si>
-    <t>SCAN CHAIN 12</t>
-  </si>
-  <si>
     <t>SCAN CHAIN 11</t>
   </si>
   <si>
@@ -872,6 +869,9 @@
   </si>
   <si>
     <t>SCAN CHAIN 1</t>
+  </si>
+  <si>
+    <t>SCAN CHAIN 0</t>
   </si>
 </sst>
 </file>
@@ -899,12 +899,18 @@
       <name val="Calibri (Corpo)"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -1030,7 +1036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1043,6 +1049,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1174,6 +1182,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC0336D9-3B55-BF4D-8BD0-C1CD54DB5E06}" name="Tabella1" displayName="Tabella1" ref="A1:C272" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
   <autoFilter ref="A1:C272" xr:uid="{CC0336D9-3B55-BF4D-8BD0-C1CD54DB5E06}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C272">
+    <sortCondition descending="1" ref="B1:B272"/>
+  </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{AF0084B7-DE3E-3D4F-AAC5-70550CC20B4E}" name="Pin Name" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{42A0CD93-E5D0-F24F-B490-26C631E422C8}" name="Index vhdl" dataDxfId="2"/>
@@ -1482,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9EBC31-E5C7-3F4F-A4B6-B9A659D71175}">
   <dimension ref="A1:C272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1491,6 +1502,7 @@
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
     <col min="3" max="3" width="59.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1506,2395 +1518,2395 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1">
+        <v>265</v>
+      </c>
+      <c r="B2" s="12">
         <v>261</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="11" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1">
+        <v>263</v>
+      </c>
+      <c r="B3" s="13">
         <v>260</v>
       </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="11" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
+        <v>262</v>
+      </c>
+      <c r="B4" s="12">
         <v>259</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="10" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
+        <v>261</v>
+      </c>
+      <c r="B5" s="13">
         <v>258</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
+        <v>260</v>
+      </c>
+      <c r="B6" s="12">
         <v>257</v>
       </c>
       <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
+        <v>259</v>
+      </c>
+      <c r="B7" s="13">
         <v>256</v>
       </c>
       <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
+        <v>258</v>
+      </c>
+      <c r="B8" s="12">
         <v>255</v>
       </c>
       <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
+        <v>257</v>
+      </c>
+      <c r="B9" s="13">
         <v>254</v>
       </c>
       <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
+        <v>256</v>
+      </c>
+      <c r="B10" s="12">
         <v>253</v>
       </c>
       <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1">
+        <v>255</v>
+      </c>
+      <c r="B11" s="13">
         <v>252</v>
       </c>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1">
+        <v>254</v>
+      </c>
+      <c r="B12" s="12">
         <v>251</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="1">
+        <v>253</v>
+      </c>
+      <c r="B13" s="13">
         <v>250</v>
       </c>
       <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1">
+        <v>252</v>
+      </c>
+      <c r="B14" s="12">
         <v>249</v>
       </c>
       <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
+        <v>251</v>
+      </c>
+      <c r="B15" s="13">
         <v>248</v>
       </c>
       <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="1">
+        <v>250</v>
+      </c>
+      <c r="B16" s="12">
         <v>247</v>
       </c>
       <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1">
+        <v>249</v>
+      </c>
+      <c r="B17" s="13">
         <v>246</v>
       </c>
       <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" s="1">
+        <v>248</v>
+      </c>
+      <c r="B18" s="12">
         <v>245</v>
       </c>
       <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="1">
+        <v>247</v>
+      </c>
+      <c r="B19" s="13">
         <v>244</v>
       </c>
       <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="1">
+        <v>246</v>
+      </c>
+      <c r="B20" s="12">
         <v>243</v>
       </c>
       <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="1">
+        <v>245</v>
+      </c>
+      <c r="B21" s="13">
         <v>242</v>
       </c>
       <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1">
+        <v>244</v>
+      </c>
+      <c r="B22" s="12">
         <v>241</v>
       </c>
       <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1">
+        <v>243</v>
+      </c>
+      <c r="B23" s="13">
         <v>240</v>
       </c>
       <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1">
+        <v>242</v>
+      </c>
+      <c r="B24" s="12">
         <v>239</v>
       </c>
       <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="1">
+        <v>241</v>
+      </c>
+      <c r="B25" s="13">
         <v>238</v>
       </c>
       <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="1">
+        <v>240</v>
+      </c>
+      <c r="B26" s="12">
         <v>237</v>
       </c>
       <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="1">
+        <v>239</v>
+      </c>
+      <c r="B27" s="13">
         <v>236</v>
       </c>
       <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28" s="1">
+        <v>238</v>
+      </c>
+      <c r="B28" s="12">
         <v>235</v>
       </c>
       <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="1">
+        <v>237</v>
+      </c>
+      <c r="B29" s="13">
         <v>234</v>
       </c>
       <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="1">
+        <v>236</v>
+      </c>
+      <c r="B30" s="12">
         <v>233</v>
       </c>
       <c r="C30" s="6"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="1">
+        <v>235</v>
+      </c>
+      <c r="B31" s="13">
         <v>232</v>
       </c>
       <c r="C31" s="6"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="1">
+        <v>234</v>
+      </c>
+      <c r="B32" s="12">
         <v>231</v>
       </c>
       <c r="C32" s="6"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33" s="1">
+        <v>233</v>
+      </c>
+      <c r="B33" s="13">
         <v>230</v>
       </c>
       <c r="C33" s="6"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="1">
+        <v>232</v>
+      </c>
+      <c r="B34" s="12">
         <v>229</v>
       </c>
       <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="1">
+        <v>231</v>
+      </c>
+      <c r="B35" s="13">
         <v>228</v>
       </c>
       <c r="C35" s="6"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="1">
+        <v>230</v>
+      </c>
+      <c r="B36" s="12">
         <v>227</v>
       </c>
       <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="1">
+        <v>229</v>
+      </c>
+      <c r="B37" s="13">
         <v>226</v>
       </c>
       <c r="C37" s="6"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="1">
+        <v>228</v>
+      </c>
+      <c r="B38" s="12">
         <v>225</v>
       </c>
       <c r="C38" s="6"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39" s="1">
+        <v>227</v>
+      </c>
+      <c r="B39" s="13">
         <v>224</v>
       </c>
       <c r="C39" s="6"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40" s="1">
+        <v>226</v>
+      </c>
+      <c r="B40" s="12">
         <v>223</v>
       </c>
       <c r="C40" s="6"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="1">
+        <v>225</v>
+      </c>
+      <c r="B41" s="13">
         <v>222</v>
       </c>
       <c r="C41" s="6"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="1">
+        <v>224</v>
+      </c>
+      <c r="B42" s="12">
         <v>221</v>
       </c>
       <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="1">
+        <v>223</v>
+      </c>
+      <c r="B43" s="13">
         <v>220</v>
       </c>
       <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" s="1">
+        <v>222</v>
+      </c>
+      <c r="B44" s="12">
         <v>219</v>
       </c>
       <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" s="1">
+        <v>221</v>
+      </c>
+      <c r="B45" s="13">
         <v>218</v>
       </c>
       <c r="C45" s="6"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B46" s="1">
+        <v>220</v>
+      </c>
+      <c r="B46" s="12">
         <v>217</v>
       </c>
       <c r="C46" s="6"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" s="1">
+        <v>219</v>
+      </c>
+      <c r="B47" s="13">
         <v>216</v>
       </c>
       <c r="C47" s="6"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B48" s="1">
+        <v>218</v>
+      </c>
+      <c r="B48" s="12">
         <v>215</v>
       </c>
       <c r="C48" s="6"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="1">
+        <v>217</v>
+      </c>
+      <c r="B49" s="13">
         <v>214</v>
       </c>
       <c r="C49" s="6"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="1">
+        <v>216</v>
+      </c>
+      <c r="B50" s="12">
         <v>213</v>
       </c>
       <c r="C50" s="6"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="1">
+        <v>215</v>
+      </c>
+      <c r="B51" s="13">
         <v>212</v>
       </c>
       <c r="C51" s="6"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B52" s="1">
+        <v>214</v>
+      </c>
+      <c r="B52" s="12">
         <v>211</v>
       </c>
       <c r="C52" s="6"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B53" s="1">
+        <v>213</v>
+      </c>
+      <c r="B53" s="13">
         <v>210</v>
       </c>
       <c r="C53" s="6"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B54" s="1">
+        <v>212</v>
+      </c>
+      <c r="B54" s="12">
         <v>209</v>
       </c>
       <c r="C54" s="6"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B55" s="1">
+        <v>211</v>
+      </c>
+      <c r="B55" s="13">
         <v>208</v>
       </c>
       <c r="C55" s="6"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B56" s="1">
+        <v>210</v>
+      </c>
+      <c r="B56" s="12">
         <v>207</v>
       </c>
       <c r="C56" s="6"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B57" s="1">
+        <v>209</v>
+      </c>
+      <c r="B57" s="13">
         <v>206</v>
       </c>
       <c r="C57" s="6"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B58" s="1">
+        <v>208</v>
+      </c>
+      <c r="B58" s="12">
         <v>205</v>
       </c>
       <c r="C58" s="6"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B59" s="1">
+        <v>207</v>
+      </c>
+      <c r="B59" s="13">
         <v>204</v>
       </c>
       <c r="C59" s="6"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" s="1">
+        <v>206</v>
+      </c>
+      <c r="B60" s="12">
         <v>203</v>
       </c>
       <c r="C60" s="6"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B61" s="1">
+        <v>205</v>
+      </c>
+      <c r="B61" s="13">
         <v>202</v>
       </c>
       <c r="C61" s="6"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B62" s="1">
+        <v>204</v>
+      </c>
+      <c r="B62" s="12">
         <v>201</v>
       </c>
       <c r="C62" s="6"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B63" s="1">
+        <v>203</v>
+      </c>
+      <c r="B63" s="13">
         <v>200</v>
       </c>
       <c r="C63" s="6"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" s="1">
+        <v>202</v>
+      </c>
+      <c r="B64" s="12">
         <v>199</v>
       </c>
       <c r="C64" s="6"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B65" s="1">
+        <v>201</v>
+      </c>
+      <c r="B65" s="13">
         <v>198</v>
       </c>
       <c r="C65" s="6"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B66" s="1">
+        <v>200</v>
+      </c>
+      <c r="B66" s="12">
         <v>197</v>
       </c>
       <c r="C66" s="6"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B67" s="1">
+        <v>199</v>
+      </c>
+      <c r="B67" s="13">
         <v>196</v>
       </c>
       <c r="C67" s="6"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B68" s="1">
+        <v>198</v>
+      </c>
+      <c r="B68" s="12">
         <v>195</v>
       </c>
       <c r="C68" s="6"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" s="1">
+        <v>197</v>
+      </c>
+      <c r="B69" s="13">
         <v>194</v>
       </c>
       <c r="C69" s="6"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B70" s="1">
+        <v>196</v>
+      </c>
+      <c r="B70" s="12">
         <v>193</v>
       </c>
       <c r="C70" s="6"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B71" s="1">
+        <v>195</v>
+      </c>
+      <c r="B71" s="13">
         <v>192</v>
       </c>
       <c r="C71" s="6"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B72" s="1">
+        <v>194</v>
+      </c>
+      <c r="B72" s="12">
         <v>191</v>
       </c>
       <c r="C72" s="6"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B73" s="1">
+        <v>193</v>
+      </c>
+      <c r="B73" s="13">
         <v>190</v>
       </c>
-      <c r="C73" s="10" t="s">
-        <v>264</v>
-      </c>
+      <c r="C73" s="6"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B74" s="1">
+        <v>192</v>
+      </c>
+      <c r="B74" s="12">
         <v>189</v>
       </c>
-      <c r="C74" s="10" t="s">
-        <v>266</v>
-      </c>
+      <c r="C74" s="6"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B75" s="1">
+        <v>191</v>
+      </c>
+      <c r="B75" s="13">
         <v>188</v>
       </c>
       <c r="C75" s="6"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B76" s="1">
+        <v>190</v>
+      </c>
+      <c r="B76" s="12">
         <v>187</v>
       </c>
       <c r="C76" s="6"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B77" s="1">
+        <v>189</v>
+      </c>
+      <c r="B77" s="13">
         <v>186</v>
       </c>
       <c r="C77" s="6"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B78" s="1">
+        <v>188</v>
+      </c>
+      <c r="B78" s="12">
         <v>185</v>
       </c>
       <c r="C78" s="6"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B79" s="1">
+        <v>187</v>
+      </c>
+      <c r="B79" s="13">
         <v>184</v>
       </c>
       <c r="C79" s="6"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B80" s="1">
+        <v>186</v>
+      </c>
+      <c r="B80" s="12">
         <v>183</v>
       </c>
       <c r="C80" s="6"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B81" s="1">
+        <v>185</v>
+      </c>
+      <c r="B81" s="13">
         <v>182</v>
       </c>
       <c r="C81" s="6"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B82" s="1">
+        <v>184</v>
+      </c>
+      <c r="B82" s="12">
         <v>181</v>
       </c>
       <c r="C82" s="6"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B83" s="1">
+        <v>183</v>
+      </c>
+      <c r="B83" s="13">
         <v>180</v>
       </c>
       <c r="C83" s="6"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B84" s="1">
+        <v>182</v>
+      </c>
+      <c r="B84" s="12">
         <v>179</v>
       </c>
       <c r="C84" s="6"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B85" s="1">
+        <v>181</v>
+      </c>
+      <c r="B85" s="13">
         <v>178</v>
       </c>
       <c r="C85" s="6"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B86" s="1">
+        <v>180</v>
+      </c>
+      <c r="B86" s="12">
         <v>177</v>
       </c>
       <c r="C86" s="6"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B87" s="1">
+        <v>179</v>
+      </c>
+      <c r="B87" s="13">
         <v>176</v>
       </c>
       <c r="C87" s="6"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B88" s="1">
+        <v>178</v>
+      </c>
+      <c r="B88" s="12">
         <v>175</v>
       </c>
       <c r="C88" s="6"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B89" s="1">
+        <v>177</v>
+      </c>
+      <c r="B89" s="13">
         <v>174</v>
       </c>
       <c r="C89" s="6"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B90" s="1">
+        <v>176</v>
+      </c>
+      <c r="B90" s="12">
         <v>173</v>
       </c>
       <c r="C90" s="6"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B91" s="1">
+        <v>175</v>
+      </c>
+      <c r="B91" s="13">
         <v>172</v>
       </c>
       <c r="C91" s="6"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B92" s="1">
+        <v>174</v>
+      </c>
+      <c r="B92" s="12">
         <v>171</v>
       </c>
       <c r="C92" s="6"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B93" s="1">
+        <v>173</v>
+      </c>
+      <c r="B93" s="13">
         <v>170</v>
       </c>
       <c r="C93" s="6"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B94" s="1">
+        <v>172</v>
+      </c>
+      <c r="B94" s="12">
         <v>169</v>
       </c>
       <c r="C94" s="6"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B95" s="1">
+        <v>171</v>
+      </c>
+      <c r="B95" s="13">
         <v>168</v>
       </c>
       <c r="C95" s="6"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B96" s="1">
+        <v>170</v>
+      </c>
+      <c r="B96" s="12">
         <v>167</v>
       </c>
       <c r="C96" s="6"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B97" s="1">
+        <v>169</v>
+      </c>
+      <c r="B97" s="13">
         <v>166</v>
       </c>
       <c r="C97" s="6"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="B98" s="1">
+        <v>168</v>
+      </c>
+      <c r="B98" s="12">
         <v>165</v>
       </c>
       <c r="C98" s="6"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B99" s="1">
+        <v>167</v>
+      </c>
+      <c r="B99" s="13">
         <v>164</v>
       </c>
       <c r="C99" s="6"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B100" s="1">
+        <v>166</v>
+      </c>
+      <c r="B100" s="12">
         <v>163</v>
       </c>
       <c r="C100" s="6"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="B101" s="1">
+        <v>165</v>
+      </c>
+      <c r="B101" s="13">
         <v>162</v>
       </c>
       <c r="C101" s="6"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B102" s="1">
+        <v>164</v>
+      </c>
+      <c r="B102" s="12">
         <v>161</v>
       </c>
       <c r="C102" s="6"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B103" s="1">
+        <v>163</v>
+      </c>
+      <c r="B103" s="13">
         <v>160</v>
       </c>
       <c r="C103" s="6"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B104" s="1">
+        <v>162</v>
+      </c>
+      <c r="B104" s="12">
         <v>159</v>
       </c>
       <c r="C104" s="6"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B105" s="1">
+        <v>161</v>
+      </c>
+      <c r="B105" s="13">
         <v>158</v>
       </c>
       <c r="C105" s="6"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="B106" s="1">
+        <v>160</v>
+      </c>
+      <c r="B106" s="12">
         <v>157</v>
       </c>
       <c r="C106" s="6"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B107" s="1">
+        <v>159</v>
+      </c>
+      <c r="B107" s="13">
         <v>156</v>
       </c>
       <c r="C107" s="6"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B108" s="1">
+        <v>158</v>
+      </c>
+      <c r="B108" s="12">
         <v>155</v>
       </c>
       <c r="C108" s="6"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B109" s="1">
+        <v>157</v>
+      </c>
+      <c r="B109" s="13">
         <v>154</v>
       </c>
       <c r="C109" s="6"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="B110" s="1">
+        <v>156</v>
+      </c>
+      <c r="B110" s="12">
         <v>153</v>
       </c>
-      <c r="C110" s="6"/>
+      <c r="C110" s="6" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B111" s="1">
+        <v>155</v>
+      </c>
+      <c r="B111" s="13">
         <v>152</v>
       </c>
-      <c r="C111" s="6"/>
+      <c r="C111" s="6" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B112" s="1">
+        <v>154</v>
+      </c>
+      <c r="B112" s="12">
         <v>151</v>
       </c>
-      <c r="C112" s="6"/>
+      <c r="C112" s="6" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="B113" s="1">
+        <v>153</v>
+      </c>
+      <c r="B113" s="13">
         <v>150</v>
       </c>
-      <c r="C113" s="6"/>
+      <c r="C113" s="6" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="B114" s="1">
+        <v>152</v>
+      </c>
+      <c r="B114" s="12">
         <v>149</v>
       </c>
-      <c r="C114" s="6"/>
+      <c r="C114" s="6" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="B115" s="1">
+        <v>151</v>
+      </c>
+      <c r="B115" s="13">
         <v>148</v>
       </c>
-      <c r="C115" s="6"/>
+      <c r="C115" s="6" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="B116" s="1">
+        <v>150</v>
+      </c>
+      <c r="B116" s="12">
         <v>147</v>
       </c>
-      <c r="C116" s="6"/>
+      <c r="C116" s="6" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B117" s="1">
+        <v>149</v>
+      </c>
+      <c r="B117" s="13">
         <v>146</v>
       </c>
-      <c r="C117" s="6"/>
+      <c r="C117" s="6" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B118" s="1">
+        <v>148</v>
+      </c>
+      <c r="B118" s="12">
         <v>145</v>
       </c>
       <c r="C118" s="6"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="B119" s="1">
+        <v>147</v>
+      </c>
+      <c r="B119" s="13">
         <v>144</v>
       </c>
-      <c r="C119" s="6"/>
+      <c r="C119" s="6" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="B120" s="1">
+        <v>146</v>
+      </c>
+      <c r="B120" s="12">
         <v>143</v>
       </c>
-      <c r="C120" s="6"/>
+      <c r="C120" s="6" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="B121" s="1">
+        <v>145</v>
+      </c>
+      <c r="B121" s="13">
         <v>142</v>
       </c>
-      <c r="C121" s="6"/>
+      <c r="C121" s="6" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="B122" s="1">
+        <v>144</v>
+      </c>
+      <c r="B122" s="12">
         <v>141</v>
       </c>
-      <c r="C122" s="6"/>
+      <c r="C122" s="6" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B123" s="1">
+        <v>143</v>
+      </c>
+      <c r="B123" s="13">
         <v>140</v>
       </c>
       <c r="C123" s="6"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="B124" s="1">
+        <v>142</v>
+      </c>
+      <c r="B124" s="12">
         <v>139</v>
       </c>
       <c r="C124" s="6"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B125" s="1">
+        <v>141</v>
+      </c>
+      <c r="B125" s="13">
         <v>138</v>
       </c>
       <c r="C125" s="6"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B126" s="1">
+        <v>140</v>
+      </c>
+      <c r="B126" s="12">
         <v>137</v>
       </c>
       <c r="C126" s="6"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B127" s="1">
+        <v>139</v>
+      </c>
+      <c r="B127" s="13">
         <v>136</v>
       </c>
       <c r="C127" s="6"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="B128" s="1">
+        <v>138</v>
+      </c>
+      <c r="B128" s="12">
         <v>135</v>
       </c>
       <c r="C128" s="6"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B129" s="1">
+        <v>137</v>
+      </c>
+      <c r="B129" s="13">
         <v>134</v>
       </c>
       <c r="C129" s="6"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B130" s="1">
+        <v>136</v>
+      </c>
+      <c r="B130" s="12">
         <v>133</v>
       </c>
       <c r="C130" s="6"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="B131" s="1">
+        <v>135</v>
+      </c>
+      <c r="B131" s="13">
         <v>132</v>
       </c>
       <c r="C131" s="6"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="B132" s="1">
+        <v>134</v>
+      </c>
+      <c r="B132" s="12">
         <v>131</v>
       </c>
       <c r="C132" s="6"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="B133" s="1">
+        <v>133</v>
+      </c>
+      <c r="B133" s="13">
         <v>130</v>
       </c>
       <c r="C133" s="6"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B134" s="1">
+        <v>132</v>
+      </c>
+      <c r="B134" s="12">
         <v>129</v>
       </c>
       <c r="C134" s="6"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B135" s="1">
+        <v>131</v>
+      </c>
+      <c r="B135" s="13">
         <v>128</v>
       </c>
       <c r="C135" s="6"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="B136" s="1">
+        <v>130</v>
+      </c>
+      <c r="B136" s="12">
         <v>127</v>
       </c>
       <c r="C136" s="6"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B137" s="1">
+        <v>129</v>
+      </c>
+      <c r="B137" s="13">
         <v>126</v>
       </c>
       <c r="C137" s="6"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B138" s="1">
+        <v>128</v>
+      </c>
+      <c r="B138" s="12">
         <v>125</v>
       </c>
       <c r="C138" s="6"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="B139" s="1">
+        <v>127</v>
+      </c>
+      <c r="B139" s="13">
         <v>124</v>
       </c>
       <c r="C139" s="6"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="B140" s="1">
+        <v>126</v>
+      </c>
+      <c r="B140" s="12">
         <v>123</v>
       </c>
       <c r="C140" s="6"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B141" s="1">
+        <v>125</v>
+      </c>
+      <c r="B141" s="13">
         <v>122</v>
       </c>
       <c r="C141" s="6"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B142" s="1">
+        <v>124</v>
+      </c>
+      <c r="B142" s="12">
         <v>121</v>
       </c>
       <c r="C142" s="6"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="B143" s="1">
+        <v>123</v>
+      </c>
+      <c r="B143" s="13">
         <v>120</v>
       </c>
       <c r="C143" s="6"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B144" s="1">
+        <v>122</v>
+      </c>
+      <c r="B144" s="12">
         <v>119</v>
       </c>
-      <c r="C144" s="6" t="s">
-        <v>279</v>
-      </c>
+      <c r="C144" s="6"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="B145" s="1">
+        <v>121</v>
+      </c>
+      <c r="B145" s="13">
         <v>118</v>
       </c>
-      <c r="C145" s="6" t="s">
-        <v>278</v>
-      </c>
+      <c r="C145" s="6"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B146" s="1">
+        <v>120</v>
+      </c>
+      <c r="B146" s="12">
         <v>117</v>
       </c>
-      <c r="C146" s="6" t="s">
-        <v>277</v>
-      </c>
+      <c r="C146" s="6"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B147" s="1">
+        <v>119</v>
+      </c>
+      <c r="B147" s="13">
         <v>116</v>
       </c>
-      <c r="C147" s="6" t="s">
-        <v>276</v>
-      </c>
+      <c r="C147" s="6"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="B148" s="1">
+        <v>118</v>
+      </c>
+      <c r="B148" s="12">
         <v>115</v>
       </c>
-      <c r="C148" s="6" t="s">
-        <v>275</v>
-      </c>
+      <c r="C148" s="6"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="B149" s="1">
+        <v>117</v>
+      </c>
+      <c r="B149" s="13">
         <v>114</v>
       </c>
-      <c r="C149" s="6" t="s">
-        <v>274</v>
-      </c>
+      <c r="C149" s="6"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B150" s="1">
+        <v>116</v>
+      </c>
+      <c r="B150" s="12">
         <v>113</v>
       </c>
-      <c r="C150" s="6" t="s">
-        <v>273</v>
-      </c>
+      <c r="C150" s="6"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B151" s="1">
+        <v>115</v>
+      </c>
+      <c r="B151" s="13">
         <v>112</v>
       </c>
-      <c r="C151" s="6" t="s">
-        <v>272</v>
-      </c>
+      <c r="C151" s="6"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B152" s="1">
+        <v>114</v>
+      </c>
+      <c r="B152" s="12">
         <v>111</v>
       </c>
-      <c r="C152" s="6" t="s">
-        <v>271</v>
-      </c>
+      <c r="C152" s="6"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B153" s="1">
+        <v>113</v>
+      </c>
+      <c r="B153" s="13">
         <v>110</v>
       </c>
-      <c r="C153" s="6" t="s">
-        <v>270</v>
-      </c>
+      <c r="C153" s="6"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B154" s="1">
+        <v>112</v>
+      </c>
+      <c r="B154" s="12">
         <v>109</v>
       </c>
-      <c r="C154" s="6" t="s">
-        <v>269</v>
-      </c>
+      <c r="C154" s="6"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="B155" s="1">
+        <v>111</v>
+      </c>
+      <c r="B155" s="13">
         <v>108</v>
       </c>
-      <c r="C155" s="6" t="s">
-        <v>268</v>
-      </c>
+      <c r="C155" s="6"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="B156" s="1">
+        <v>110</v>
+      </c>
+      <c r="B156" s="12">
         <v>107</v>
       </c>
       <c r="C156" s="6"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="B157" s="1">
+        <v>109</v>
+      </c>
+      <c r="B157" s="13">
         <v>106</v>
       </c>
       <c r="C157" s="6"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B158" s="1">
+        <v>108</v>
+      </c>
+      <c r="B158" s="12">
         <v>105</v>
       </c>
       <c r="C158" s="6"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B159" s="1">
+        <v>107</v>
+      </c>
+      <c r="B159" s="13">
         <v>104</v>
       </c>
       <c r="C159" s="6"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B160" s="1">
+        <v>106</v>
+      </c>
+      <c r="B160" s="12">
         <v>103</v>
       </c>
       <c r="C160" s="6"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="B161" s="1">
+        <v>105</v>
+      </c>
+      <c r="B161" s="13">
         <v>102</v>
       </c>
       <c r="C161" s="6"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="B162" s="1">
+        <v>104</v>
+      </c>
+      <c r="B162" s="12">
         <v>101</v>
       </c>
       <c r="C162" s="6"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="B163" s="1">
+        <v>103</v>
+      </c>
+      <c r="B163" s="13">
         <v>100</v>
       </c>
       <c r="C163" s="6"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="B164" s="1">
+        <v>102</v>
+      </c>
+      <c r="B164" s="12">
         <v>99</v>
       </c>
       <c r="C164" s="6"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B165" s="1">
+        <v>101</v>
+      </c>
+      <c r="B165" s="13">
         <v>98</v>
       </c>
       <c r="C165" s="6"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="B166" s="1">
+        <v>100</v>
+      </c>
+      <c r="B166" s="12">
         <v>97</v>
       </c>
       <c r="C166" s="6"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B167" s="1">
+        <v>99</v>
+      </c>
+      <c r="B167" s="13">
         <v>96</v>
       </c>
       <c r="C167" s="6"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B168" s="1">
+        <v>98</v>
+      </c>
+      <c r="B168" s="12">
         <v>95</v>
       </c>
       <c r="C168" s="6"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B169" s="1">
+        <v>97</v>
+      </c>
+      <c r="B169" s="13">
         <v>94</v>
       </c>
       <c r="C169" s="6"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B170" s="1">
+        <v>96</v>
+      </c>
+      <c r="B170" s="12">
         <v>93</v>
       </c>
       <c r="C170" s="6"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B171" s="1">
+        <v>95</v>
+      </c>
+      <c r="B171" s="13">
         <v>92</v>
       </c>
       <c r="C171" s="6"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="B172" s="1">
+        <v>94</v>
+      </c>
+      <c r="B172" s="12">
         <v>91</v>
       </c>
       <c r="C172" s="6"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B173" s="1">
+        <v>93</v>
+      </c>
+      <c r="B173" s="13">
         <v>90</v>
       </c>
       <c r="C173" s="6"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="B174" s="1">
+        <v>92</v>
+      </c>
+      <c r="B174" s="12">
         <v>89</v>
       </c>
       <c r="C174" s="6"/>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B175" s="1">
+        <v>91</v>
+      </c>
+      <c r="B175" s="13">
         <v>88</v>
       </c>
       <c r="C175" s="6"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B176" s="1">
+        <v>90</v>
+      </c>
+      <c r="B176" s="12">
         <v>87</v>
       </c>
       <c r="C176" s="6"/>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="B177" s="1">
+        <v>89</v>
+      </c>
+      <c r="B177" s="13">
         <v>86</v>
       </c>
       <c r="C177" s="6"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="B178" s="1">
+        <v>88</v>
+      </c>
+      <c r="B178" s="12">
         <v>85</v>
       </c>
       <c r="C178" s="6"/>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="B179" s="1">
+        <v>87</v>
+      </c>
+      <c r="B179" s="13">
         <v>84</v>
       </c>
       <c r="C179" s="6"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B180" s="1">
+        <v>86</v>
+      </c>
+      <c r="B180" s="12">
         <v>83</v>
       </c>
       <c r="C180" s="6"/>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="B181" s="1">
+        <v>85</v>
+      </c>
+      <c r="B181" s="13">
         <v>82</v>
       </c>
       <c r="C181" s="6"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="B182" s="1">
+        <v>84</v>
+      </c>
+      <c r="B182" s="12">
         <v>81</v>
       </c>
       <c r="C182" s="6"/>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B183" s="1">
+        <v>83</v>
+      </c>
+      <c r="B183" s="13">
         <v>80</v>
       </c>
       <c r="C183" s="6"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B184" s="1">
+        <v>82</v>
+      </c>
+      <c r="B184" s="12">
         <v>79</v>
       </c>
       <c r="C184" s="6"/>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="B185" s="1">
+        <v>81</v>
+      </c>
+      <c r="B185" s="13">
         <v>78</v>
       </c>
       <c r="C185" s="6"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="B186" s="1">
+        <v>80</v>
+      </c>
+      <c r="B186" s="12">
         <v>77</v>
       </c>
       <c r="C186" s="6"/>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="B187" s="1">
+        <v>79</v>
+      </c>
+      <c r="B187" s="13">
         <v>76</v>
       </c>
       <c r="C187" s="6"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="B188" s="1">
+        <v>78</v>
+      </c>
+      <c r="B188" s="12">
         <v>75</v>
       </c>
       <c r="C188" s="6"/>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="B189" s="1">
+        <v>77</v>
+      </c>
+      <c r="B189" s="13">
         <v>74</v>
       </c>
       <c r="C189" s="6"/>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="B190" s="1">
+        <v>76</v>
+      </c>
+      <c r="B190" s="12">
         <v>73</v>
       </c>
       <c r="C190" s="6"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="B191" s="1">
+        <v>75</v>
+      </c>
+      <c r="B191" s="13">
         <v>72</v>
       </c>
-      <c r="C191" s="6"/>
+      <c r="C191" s="10" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="B192" s="1">
+        <v>74</v>
+      </c>
+      <c r="B192" s="12">
         <v>71</v>
       </c>
-      <c r="C192" s="6"/>
+      <c r="C192" s="10" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="B193" s="1">
+        <v>73</v>
+      </c>
+      <c r="B193" s="13">
         <v>70</v>
       </c>
       <c r="C193" s="6"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="B194" s="1">
+        <v>72</v>
+      </c>
+      <c r="B194" s="12">
         <v>69</v>
       </c>
       <c r="C194" s="6"/>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="B195" s="1">
+        <v>71</v>
+      </c>
+      <c r="B195" s="13">
         <v>68</v>
       </c>
       <c r="C195" s="6"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="B196" s="1">
+        <v>70</v>
+      </c>
+      <c r="B196" s="12">
         <v>67</v>
       </c>
       <c r="C196" s="6"/>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="B197" s="1">
+        <v>69</v>
+      </c>
+      <c r="B197" s="13">
         <v>66</v>
       </c>
       <c r="C197" s="6"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="B198" s="1">
+        <v>68</v>
+      </c>
+      <c r="B198" s="12">
         <v>65</v>
       </c>
       <c r="C198" s="6"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="B199" s="1">
+        <v>67</v>
+      </c>
+      <c r="B199" s="13">
         <v>64</v>
       </c>
       <c r="C199" s="6"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B200" s="1">
+        <v>66</v>
+      </c>
+      <c r="B200" s="12">
         <v>63</v>
       </c>
       <c r="C200" s="6"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" s="5" t="s">
-        <v>202</v>
-      </c>
-      <c r="B201" s="1">
+        <v>65</v>
+      </c>
+      <c r="B201" s="13">
         <v>62</v>
       </c>
       <c r="C201" s="6"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="B202" s="1">
+        <v>64</v>
+      </c>
+      <c r="B202" s="12">
         <v>61</v>
       </c>
       <c r="C202" s="6"/>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="B203" s="1">
+        <v>63</v>
+      </c>
+      <c r="B203" s="13">
         <v>60</v>
       </c>
       <c r="C203" s="6"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B204" s="1">
+        <v>62</v>
+      </c>
+      <c r="B204" s="12">
         <v>59</v>
       </c>
       <c r="C204" s="6"/>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="B205" s="1">
+        <v>61</v>
+      </c>
+      <c r="B205" s="13">
         <v>58</v>
       </c>
       <c r="C205" s="6"/>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="B206" s="1">
+        <v>60</v>
+      </c>
+      <c r="B206" s="12">
         <v>57</v>
       </c>
       <c r="C206" s="6"/>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="B207" s="1">
+        <v>59</v>
+      </c>
+      <c r="B207" s="13">
         <v>56</v>
       </c>
       <c r="C207" s="6"/>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="B208" s="1">
+        <v>58</v>
+      </c>
+      <c r="B208" s="12">
         <v>55</v>
       </c>
       <c r="C208" s="6"/>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="B209" s="1">
+        <v>57</v>
+      </c>
+      <c r="B209" s="13">
         <v>54</v>
       </c>
       <c r="C209" s="6"/>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="B210" s="1">
+        <v>56</v>
+      </c>
+      <c r="B210" s="12">
         <v>53</v>
       </c>
       <c r="C210" s="6"/>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B211" s="1">
+        <v>55</v>
+      </c>
+      <c r="B211" s="13">
         <v>52</v>
       </c>
       <c r="C211" s="6"/>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="B212" s="1">
+        <v>54</v>
+      </c>
+      <c r="B212" s="12">
         <v>51</v>
       </c>
       <c r="C212" s="6"/>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="B213" s="1">
+        <v>53</v>
+      </c>
+      <c r="B213" s="13">
         <v>50</v>
       </c>
       <c r="C213" s="6"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B214" s="1">
+        <v>52</v>
+      </c>
+      <c r="B214" s="12">
         <v>49</v>
       </c>
       <c r="C214" s="6"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="B215" s="1">
+        <v>51</v>
+      </c>
+      <c r="B215" s="13">
         <v>48</v>
       </c>
       <c r="C215" s="6"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="B216" s="1">
+        <v>50</v>
+      </c>
+      <c r="B216" s="12">
         <v>47</v>
       </c>
       <c r="C216" s="6"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="B217" s="1">
+        <v>49</v>
+      </c>
+      <c r="B217" s="13">
         <v>46</v>
       </c>
       <c r="C217" s="6"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B218" s="1">
+        <v>48</v>
+      </c>
+      <c r="B218" s="12">
         <v>45</v>
       </c>
       <c r="C218" s="6"/>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="B219" s="1">
+        <v>47</v>
+      </c>
+      <c r="B219" s="13">
         <v>44</v>
       </c>
       <c r="C219" s="6"/>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A220" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="B220" s="1">
+        <v>46</v>
+      </c>
+      <c r="B220" s="12">
         <v>43</v>
       </c>
       <c r="C220" s="6"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="B221" s="1">
+        <v>45</v>
+      </c>
+      <c r="B221" s="13">
         <v>42</v>
       </c>
       <c r="C221" s="6"/>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A222" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="B222" s="1">
+        <v>44</v>
+      </c>
+      <c r="B222" s="12">
         <v>41</v>
       </c>
       <c r="C222" s="6"/>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="B223" s="1">
+        <v>43</v>
+      </c>
+      <c r="B223" s="13">
         <v>40</v>
       </c>
       <c r="C223" s="6"/>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="B224" s="1">
+        <v>42</v>
+      </c>
+      <c r="B224" s="12">
         <v>39</v>
       </c>
       <c r="C224" s="6"/>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="B225" s="1">
+        <v>41</v>
+      </c>
+      <c r="B225" s="13">
         <v>38</v>
       </c>
       <c r="C225" s="6"/>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B226" s="1">
+        <v>40</v>
+      </c>
+      <c r="B226" s="12">
         <v>37</v>
       </c>
       <c r="C226" s="6"/>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="5" t="s">
-        <v>228</v>
-      </c>
-      <c r="B227" s="1">
+        <v>39</v>
+      </c>
+      <c r="B227" s="13">
         <v>36</v>
       </c>
       <c r="C227" s="6"/>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="B228" s="1">
+        <v>38</v>
+      </c>
+      <c r="B228" s="12">
         <v>35</v>
       </c>
       <c r="C228" s="6"/>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="B229" s="1">
+        <v>37</v>
+      </c>
+      <c r="B229" s="13">
         <v>34</v>
       </c>
       <c r="C229" s="6"/>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="B230" s="1">
+        <v>36</v>
+      </c>
+      <c r="B230" s="12">
         <v>33</v>
       </c>
       <c r="C230" s="6"/>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="B231" s="1">
+        <v>35</v>
+      </c>
+      <c r="B231" s="13">
         <v>32</v>
       </c>
       <c r="C231" s="6"/>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="B232" s="1">
+        <v>34</v>
+      </c>
+      <c r="B232" s="12">
         <v>31</v>
       </c>
       <c r="C232" s="6"/>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="B233" s="1">
+        <v>33</v>
+      </c>
+      <c r="B233" s="13">
         <v>30</v>
       </c>
       <c r="C233" s="6"/>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="B234" s="1">
+        <v>32</v>
+      </c>
+      <c r="B234" s="12">
         <v>29</v>
       </c>
       <c r="C234" s="6"/>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B235" s="1">
+        <v>31</v>
+      </c>
+      <c r="B235" s="13">
         <v>28</v>
       </c>
       <c r="C235" s="6"/>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="B236" s="1">
+        <v>30</v>
+      </c>
+      <c r="B236" s="12">
         <v>27</v>
       </c>
       <c r="C236" s="6"/>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="B237" s="1">
+        <v>29</v>
+      </c>
+      <c r="B237" s="13">
         <v>26</v>
       </c>
       <c r="C237" s="6"/>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="B238" s="1">
+        <v>28</v>
+      </c>
+      <c r="B238" s="12">
         <v>25</v>
       </c>
       <c r="C238" s="6"/>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="B239" s="1">
+        <v>27</v>
+      </c>
+      <c r="B239" s="13">
         <v>24</v>
       </c>
       <c r="C239" s="6"/>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="B240" s="1">
+        <v>26</v>
+      </c>
+      <c r="B240" s="12">
         <v>23</v>
       </c>
       <c r="C240" s="6"/>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="B241" s="1">
+        <v>25</v>
+      </c>
+      <c r="B241" s="13">
         <v>22</v>
       </c>
       <c r="C241" s="6"/>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="B242" s="1">
+        <v>24</v>
+      </c>
+      <c r="B242" s="12">
         <v>21</v>
       </c>
       <c r="C242" s="6"/>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="B243" s="1">
+        <v>23</v>
+      </c>
+      <c r="B243" s="13">
         <v>20</v>
       </c>
       <c r="C243" s="6"/>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="B244" s="1">
+        <v>22</v>
+      </c>
+      <c r="B244" s="12">
         <v>19</v>
       </c>
       <c r="C244" s="6"/>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B245" s="1">
+        <v>21</v>
+      </c>
+      <c r="B245" s="13">
         <v>18</v>
       </c>
       <c r="C245" s="6"/>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="B246" s="1">
+        <v>20</v>
+      </c>
+      <c r="B246" s="12">
         <v>17</v>
       </c>
       <c r="C246" s="6"/>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="B247" s="1">
+        <v>19</v>
+      </c>
+      <c r="B247" s="13">
         <v>16</v>
       </c>
       <c r="C247" s="6"/>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B248" s="1">
+        <v>18</v>
+      </c>
+      <c r="B248" s="12">
         <v>15</v>
       </c>
       <c r="C248" s="6"/>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="B249" s="1">
+        <v>17</v>
+      </c>
+      <c r="B249" s="13">
         <v>14</v>
       </c>
       <c r="C249" s="6"/>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="B250" s="1">
+        <v>16</v>
+      </c>
+      <c r="B250" s="12">
         <v>13</v>
       </c>
       <c r="C250" s="6"/>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="B251" s="1">
+        <v>15</v>
+      </c>
+      <c r="B251" s="13">
         <v>12</v>
       </c>
       <c r="C251" s="6"/>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="B252" s="1">
+        <v>14</v>
+      </c>
+      <c r="B252" s="12">
         <v>11</v>
       </c>
       <c r="C252" s="6"/>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="5" t="s">
-        <v>254</v>
-      </c>
-      <c r="B253" s="1">
+        <v>13</v>
+      </c>
+      <c r="B253" s="13">
         <v>10</v>
       </c>
       <c r="C253" s="6"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="B254" s="1">
+        <v>12</v>
+      </c>
+      <c r="B254" s="12">
         <v>9</v>
       </c>
       <c r="C254" s="6"/>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="B255" s="1">
+        <v>11</v>
+      </c>
+      <c r="B255" s="13">
         <v>8</v>
       </c>
       <c r="C255" s="6"/>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B256" s="1">
+        <v>10</v>
+      </c>
+      <c r="B256" s="12">
         <v>7</v>
       </c>
       <c r="C256" s="6"/>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="B257" s="1">
+        <v>9</v>
+      </c>
+      <c r="B257" s="13">
         <v>6</v>
       </c>
       <c r="C257" s="6"/>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="B258" s="1">
+        <v>8</v>
+      </c>
+      <c r="B258" s="12">
         <v>5</v>
       </c>
       <c r="C258" s="6"/>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A259" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="B259" s="1">
+        <v>7</v>
+      </c>
+      <c r="B259" s="13">
         <v>4</v>
       </c>
       <c r="C259" s="6"/>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="B260" s="1">
+        <v>6</v>
+      </c>
+      <c r="B260" s="12">
         <v>3</v>
       </c>
       <c r="C260" s="6"/>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="B261" s="1">
+        <v>5</v>
+      </c>
+      <c r="B261" s="13">
         <v>2</v>
       </c>
-      <c r="C261" s="10" t="s">
-        <v>267</v>
-      </c>
+      <c r="C261" s="6"/>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="B262" s="1">
+        <v>4</v>
+      </c>
+      <c r="B262" s="12">
         <v>1</v>
       </c>
-      <c r="C262" s="11" t="s">
-        <v>266</v>
-      </c>
+      <c r="C262" s="6"/>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="B263" s="1">
+        <v>3</v>
+      </c>
+      <c r="B263" s="13">
         <v>0</v>
       </c>
-      <c r="C263" s="11" t="s">
-        <v>266</v>
-      </c>
+      <c r="C263" s="6"/>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="5"/>

</xml_diff>

<commit_message>
FIX: few fixs in controller and memories, MOD: spf2data.tcl can provide also capture patterns
</commit_message>
<xml_diff>
--- a/bist/atpg_pat_converter/PinFunc/PIs.xlsx
+++ b/bist/atpg_pat_converter/PinFunc/PIs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luca/Documents/VirtualShared/testing/RISCV_LBIST/bist/atpg_pat_converter/PinFunc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83704488-8D73-2147-9C0F-F58510CACE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33910E8D-6712-5B4A-82A6-F0698F9B3E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{C32979EF-4B37-0B40-98B1-A31D6BD3C0AB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14380" xr2:uid="{C32979EF-4B37-0B40-98B1-A31D6BD3C0AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="281">
   <si>
     <t>Pin Name</t>
   </si>
@@ -826,18 +826,9 @@
     <t xml:space="preserve"> "test_en_i" </t>
   </si>
   <si>
-    <t>FIXED AT 'test_clk_g' in test_mode</t>
-  </si>
-  <si>
     <t xml:space="preserve"> "test_mode"</t>
   </si>
   <si>
-    <t>FIXED AT '1' during load-capture</t>
-  </si>
-  <si>
-    <t>FIXED AT 'test_rst_g' in test_mode</t>
-  </si>
-  <si>
     <t>SCAN CHAIN 11</t>
   </si>
   <si>
@@ -872,6 +863,18 @@
   </si>
   <si>
     <t>SCAN CHAIN 0</t>
+  </si>
+  <si>
+    <t>FIXED AT '1' during load/unload phase</t>
+  </si>
+  <si>
+    <t>FIXED AT 'test_rst_g' during all test</t>
+  </si>
+  <si>
+    <t>FIXED AT 'test_clk_g' during all test</t>
+  </si>
+  <si>
+    <t>CONFIGURATION: SCAN CHAINS 12, COMPRESSOR 480, MAX_SCAN_LENGTH = 8</t>
   </si>
 </sst>
 </file>
@@ -1061,24 +1064,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -1144,6 +1129,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -1158,12 +1159,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
+        <top/>
+        <bottom/>
+        <vertical style="thin">
           <color indexed="64"/>
-        </top>
-        <bottom style="thin">
+        </vertical>
+        <horizontal style="thin">
           <color indexed="64"/>
-        </bottom>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -1180,15 +1183,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC0336D9-3B55-BF4D-8BD0-C1CD54DB5E06}" name="Tabella1" displayName="Tabella1" ref="A1:C272" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC0336D9-3B55-BF4D-8BD0-C1CD54DB5E06}" name="Tabella1" displayName="Tabella1" ref="A1:C272" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A1:C272" xr:uid="{CC0336D9-3B55-BF4D-8BD0-C1CD54DB5E06}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C272">
     <sortCondition descending="1" ref="B1:B272"/>
   </sortState>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AF0084B7-DE3E-3D4F-AAC5-70550CC20B4E}" name="Pin Name" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{42A0CD93-E5D0-F24F-B490-26C631E422C8}" name="Index vhdl" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{4C9B16A5-D69E-3340-BFE5-23BC4CFB6C0C}" name="comments" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{AF0084B7-DE3E-3D4F-AAC5-70550CC20B4E}" name="Pin Name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{42A0CD93-E5D0-F24F-B490-26C631E422C8}" name="Index vhdl" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{4C9B16A5-D69E-3340-BFE5-23BC4CFB6C0C}" name="comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1491,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9EBC31-E5C7-3F4F-A4B6-B9A659D71175}">
-  <dimension ref="A1:C272"/>
+  <dimension ref="A1:E272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1502,10 +1505,11 @@
     <col min="1" max="1" width="29.1640625" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" customWidth="1"/>
     <col min="3" max="3" width="59.33203125" customWidth="1"/>
+    <col min="5" max="5" width="75.33203125" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1516,18 +1520,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B2" s="12">
         <v>261</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>263</v>
       </c>
@@ -1535,10 +1539,13 @@
         <v>260</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+      <c r="E3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>262</v>
       </c>
@@ -1546,10 +1553,10 @@
         <v>259</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>261</v>
       </c>
@@ -1558,7 +1565,7 @@
       </c>
       <c r="C5" s="6"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>260</v>
       </c>
@@ -1567,7 +1574,7 @@
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>259</v>
       </c>
@@ -1576,7 +1583,7 @@
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>258</v>
       </c>
@@ -1585,7 +1592,7 @@
       </c>
       <c r="C8" s="6"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>257</v>
       </c>
@@ -1594,7 +1601,7 @@
       </c>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>256</v>
       </c>
@@ -1603,7 +1610,7 @@
       </c>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>255</v>
       </c>
@@ -1612,7 +1619,7 @@
       </c>
       <c r="C11" s="6"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>254</v>
       </c>
@@ -1621,7 +1628,7 @@
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>253</v>
       </c>
@@ -1630,7 +1637,7 @@
       </c>
       <c r="C13" s="6"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>252</v>
       </c>
@@ -1639,7 +1646,7 @@
       </c>
       <c r="C14" s="6"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>251</v>
       </c>
@@ -1648,7 +1655,7 @@
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>250</v>
       </c>
@@ -2502,7 +2509,7 @@
         <v>153</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
@@ -2513,7 +2520,7 @@
         <v>152</v>
       </c>
       <c r="C111" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -2524,7 +2531,7 @@
         <v>151</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -2535,7 +2542,7 @@
         <v>150</v>
       </c>
       <c r="C113" s="6" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -2546,7 +2553,7 @@
         <v>149</v>
       </c>
       <c r="C114" s="6" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -2557,7 +2564,7 @@
         <v>148</v>
       </c>
       <c r="C115" s="6" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
@@ -2568,7 +2575,7 @@
         <v>147</v>
       </c>
       <c r="C116" s="6" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
@@ -2579,7 +2586,7 @@
         <v>146</v>
       </c>
       <c r="C117" s="6" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -2599,7 +2606,7 @@
         <v>144</v>
       </c>
       <c r="C119" s="6" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -2610,7 +2617,7 @@
         <v>143</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -2621,7 +2628,7 @@
         <v>142</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -2632,7 +2639,7 @@
         <v>141</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -3255,7 +3262,7 @@
         <v>72</v>
       </c>
       <c r="C191" s="10" t="s">
-        <v>266</v>
+        <v>277</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
@@ -3266,7 +3273,7 @@
         <v>71</v>
       </c>
       <c r="C192" s="10" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>